<commit_message>
Updated for new api
</commit_message>
<xml_diff>
--- a/Sentimental/bin/Debug/Book1.xlsx
+++ b/Sentimental/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rc23cbda12e4b479f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R05a027d70ec44977"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R546f093654244c44"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9d3352ddd1e44428"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ac804877-faa6-46f4-a286-757032710367}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2e3ac9cd-7dc4-458f-8f98-e3a000c37945}">
   <we:reference id="588f58d6-4f88-46ac-9a9a-0c37105e18b4" version="1.0.0.2" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Updates API key (yes i know it is open and you can steal it, but this is just a demo)
</commit_message>
<xml_diff>
--- a/Sentimental/bin/Debug/Book1.xlsx
+++ b/Sentimental/bin/Debug/Book1.xlsx
@@ -2,25 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R05a027d70ec44977"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R4008d48cef2b4993"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9d3352ddd1e44428"/>
+  <wetp:taskpane dockstate="" visibility="1" width="525" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re42c5d192c854f04"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2e3ac9cd-7dc4-458f-8f98-e3a000c37945}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{82e5098e-70fc-4c33-b8a2-75f1d9c018d0}">
   <we:reference id="588f58d6-4f88-46ac-9a9a-0c37105e18b4" version="1.0.0.2" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>
   <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
 </file>
 

</xml_diff>

<commit_message>
Updates API key (yes i know it is open and you can steal it, but this is just a demo). Also decomission notice
</commit_message>
<xml_diff>
--- a/Sentimental/bin/Debug/Book1.xlsx
+++ b/Sentimental/bin/Debug/Book1.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R4008d48cef2b4993"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdb2b85b5890c478c"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="525" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re42c5d192c854f04"/>
+  <wetp:taskpane dockstate="" visibility="1" width="700" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R72b14d453c3846f3"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{82e5098e-70fc-4c33-b8a2-75f1d9c018d0}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ed20abe3-7622-44bb-9edb-d5e8f47d5ee9}">
   <we:reference id="588f58d6-4f88-46ac-9a9a-0c37105e18b4" version="1.0.0.2" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>